<commit_message>
updating submission date to today
I typically use the run date vs. the actual submission date.
</commit_message>
<xml_diff>
--- a/results/historical/OpenStudio_BESTEST_historical.xlsx
+++ b/results/historical/OpenStudio_BESTEST_historical.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgoldwas/Documents/GitHub/NREL/BESTEST-GSR/results/historical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BD8B7A-C018-A546-94E0-C0D0379EE155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12C7ED7-DCC7-6C4D-A530-3CC7F1AB2174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB Envelope" sheetId="2" r:id="rId1"/>
@@ -6974,27 +6974,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -19937,17 +19917,17 @@
   </sheetData>
   <autoFilter ref="A1:E660" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="B1:C6 B661:C1048576">
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B660">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C660">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19963,7 +19943,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E1449" sqref="E1449"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20044,7 +20024,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>43573</v>
+        <v>43810</v>
       </c>
       <c r="E4" s="1">
         <v>43573</v>
@@ -47269,12 +47249,12 @@
   </sheetData>
   <autoFilter ref="A1:E1437" xr:uid="{3658DFBE-1F59-D443-8645-E2D1C3041DCA}"/>
   <conditionalFormatting sqref="B8:C1437 B7">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48312,22 +48292,22 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="B8:C54 B7">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C54">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C54">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C54">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C7)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>